<commit_message>
Presencas até 24/11 incluidas
</commit_message>
<xml_diff>
--- a/presencas.xlsx
+++ b/presencas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B9D62E-4187-4324-8BF4-01B8D7D56C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FFBE51-49CF-4807-AA8A-C5DB8C4ECB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,18 +16,18 @@
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respostas ao formulário 1'!$A$1:$F$2369</definedName>
-    <definedName name="Z_25BF9AEC_6AF4_40B5_9B09_EFFFE67B0424_.wvu.FilterData" localSheetId="0" hidden="1">'Respostas ao formulário 1'!$A$1:$F$2469</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respostas ao formulário 1'!$A$1:$F$2452</definedName>
+    <definedName name="Z_13F12EAD_C763_4533_AABC_1B0310D4A0A2_.wvu.FilterData" localSheetId="0" hidden="1">'Respostas ao formulário 1'!$A$1:$F$2552</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Filtro 1" guid="{25BF9AEC-6AF4-40B5-9B09-EFFFE67B0424}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filtro 1" guid="{13F12EAD-C763-4533-AABC-1B0310D4A0A2}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7111" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7360" uniqueCount="802">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2406,6 +2406,33 @@
   </si>
   <si>
     <t>Nunca. Um general."</t>
+  </si>
+  <si>
+    <t>Carreira</t>
+  </si>
+  <si>
+    <t>Nicollas Oliveira  Figueiróo</t>
+  </si>
+  <si>
+    <t>carreira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karina rodrigues de souza </t>
+  </si>
+  <si>
+    <t>GUILHERME HENRIQUE SANCHES BERNARDINO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amanda cano Jardim </t>
+  </si>
+  <si>
+    <t>SANDRO MARCELO SOARES RUGGIERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carreira </t>
+  </si>
+  <si>
+    <t>Entrevista</t>
   </si>
 </sst>
 </file>
@@ -2681,16 +2708,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F2369"/>
+  <dimension ref="A1:F2452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2344" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <pane ySplit="1" topLeftCell="A2419" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2436" sqref="D2436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="8" customWidth="1"/>
     <col min="2" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" customWidth="1"/>
     <col min="6" max="6" width="106.42578125" customWidth="1"/>
@@ -50077,12 +50104,1672 @@
         <v>447</v>
       </c>
     </row>
+    <row r="2370" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2370" s="7">
+        <v>44517.856994490736</v>
+      </c>
+      <c r="B2370" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2370" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2370" s="2">
+        <v>81727525</v>
+      </c>
+      <c r="E2370" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2370" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2371" s="7">
+        <v>44517.857204039348</v>
+      </c>
+      <c r="B2371" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2371" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2371" s="2">
+        <v>819142037</v>
+      </c>
+      <c r="E2371" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2371" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2372" s="7">
+        <v>44517.857263217593</v>
+      </c>
+      <c r="B2372" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2372" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D2372" s="2">
+        <v>82016277</v>
+      </c>
+      <c r="E2372" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2372" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2373" s="7">
+        <v>44517.857320949071</v>
+      </c>
+      <c r="B2373" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2373" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2373" s="2">
+        <v>81826339</v>
+      </c>
+      <c r="E2373" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2373" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2374" s="7">
+        <v>44517.857342939817</v>
+      </c>
+      <c r="B2374" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2374" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2374" s="2">
+        <v>818110212</v>
+      </c>
+      <c r="E2374" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2374" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2375" s="7">
+        <v>44517.857343287033</v>
+      </c>
+      <c r="B2375" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2375" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2375" s="2">
+        <v>818129658</v>
+      </c>
+      <c r="E2375" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2375" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2376" s="7">
+        <v>44517.857353553241</v>
+      </c>
+      <c r="B2376" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2376" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2376" s="2">
+        <v>818234016</v>
+      </c>
+      <c r="E2376" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2376" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2377" s="7">
+        <v>44517.857355532411</v>
+      </c>
+      <c r="B2377" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2377" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2377" s="2">
+        <v>81815561</v>
+      </c>
+      <c r="E2377" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2377" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2378" s="7">
+        <v>44517.857378206019</v>
+      </c>
+      <c r="B2378" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2378" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2378" s="2">
+        <v>81722214</v>
+      </c>
+      <c r="E2378" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2378" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2379" s="7">
+        <v>44517.857452604163</v>
+      </c>
+      <c r="B2379" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2379" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2379" s="2">
+        <v>818141547</v>
+      </c>
+      <c r="E2379" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2379" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2380" s="7">
+        <v>44517.857464166664</v>
+      </c>
+      <c r="B2380" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2380" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2380" s="2">
+        <v>81823402</v>
+      </c>
+      <c r="E2380" s="3">
+        <v>44152</v>
+      </c>
+      <c r="F2380" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2381" s="7">
+        <v>44517.85748525463</v>
+      </c>
+      <c r="B2381" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2381" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2381" s="2">
+        <v>820120772</v>
+      </c>
+      <c r="E2381" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2381" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2382" s="7">
+        <v>44517.857597025461</v>
+      </c>
+      <c r="B2382" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2382" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2382" s="2">
+        <v>818234790</v>
+      </c>
+      <c r="E2382" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2382" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2383" s="7">
+        <v>44517.857612094907</v>
+      </c>
+      <c r="B2383" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2383" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2383" s="2">
+        <v>818145466</v>
+      </c>
+      <c r="E2383" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2383" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2384" s="7">
+        <v>44517.857663414354</v>
+      </c>
+      <c r="B2384" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2384" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2384" s="2">
+        <v>818128371</v>
+      </c>
+      <c r="E2384" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2384" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2385" s="7">
+        <v>44517.857701793982</v>
+      </c>
+      <c r="B2385" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2385" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2385" s="2">
+        <v>818147528</v>
+      </c>
+      <c r="E2385" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2385" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2386" s="7">
+        <v>44517.857793634263</v>
+      </c>
+      <c r="B2386" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2386" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2386" s="2">
+        <v>81717296</v>
+      </c>
+      <c r="E2386" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2386" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2387" s="7">
+        <v>44517.857827812499</v>
+      </c>
+      <c r="B2387" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2387" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2387" s="2">
+        <v>820270845</v>
+      </c>
+      <c r="E2387" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2387" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2388" s="7">
+        <v>44517.857833182876</v>
+      </c>
+      <c r="B2388" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2388" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2388" s="2">
+        <v>81814286</v>
+      </c>
+      <c r="E2388" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2388" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2389" s="7">
+        <v>44517.857865729165</v>
+      </c>
+      <c r="B2389" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2389" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2389" s="2">
+        <v>81620106</v>
+      </c>
+      <c r="E2389" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2389" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2390" s="7">
+        <v>44517.857881354168</v>
+      </c>
+      <c r="B2390" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2390" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2390" s="2">
+        <v>818136491</v>
+      </c>
+      <c r="E2390" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2390" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2391" s="7">
+        <v>44517.857891145832</v>
+      </c>
+      <c r="B2391" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2391" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2391" s="2">
+        <v>818112270</v>
+      </c>
+      <c r="E2391" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2391" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2392" s="7">
+        <v>44517.857898391201</v>
+      </c>
+      <c r="B2392" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2392" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2392" s="2">
+        <v>818149040</v>
+      </c>
+      <c r="E2392" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2392" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2393" s="7">
+        <v>44517.857974872684</v>
+      </c>
+      <c r="B2393" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2393" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2393" s="2">
+        <v>816114969</v>
+      </c>
+      <c r="E2393" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2393" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2394" s="7">
+        <v>44517.857976747684</v>
+      </c>
+      <c r="B2394" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2394" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D2394" s="2">
+        <v>818136575</v>
+      </c>
+      <c r="E2394" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2394" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2395" s="7">
+        <v>44517.858017928243</v>
+      </c>
+      <c r="B2395" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2395" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2395" s="2">
+        <v>819225204</v>
+      </c>
+      <c r="E2395" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2395" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2396" s="7">
+        <v>44517.858082893523</v>
+      </c>
+      <c r="B2396" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2396" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2396" s="2">
+        <v>818231417</v>
+      </c>
+      <c r="E2396" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2396" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2397" s="7">
+        <v>44517.858110567133</v>
+      </c>
+      <c r="B2397" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2397" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2397" s="2">
+        <v>819228006</v>
+      </c>
+      <c r="E2397" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2397" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2398" s="7">
+        <v>44517.858218576388</v>
+      </c>
+      <c r="B2398" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2398" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2398" s="2">
+        <v>81820360</v>
+      </c>
+      <c r="E2398" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2398" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2399" s="7">
+        <v>44517.858325717592</v>
+      </c>
+      <c r="B2399" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2399" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2399" s="2">
+        <v>81823608</v>
+      </c>
+      <c r="E2399" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2399" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2400" s="7">
+        <v>44517.858348645837</v>
+      </c>
+      <c r="B2400" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2400" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2400" s="2">
+        <v>817122831</v>
+      </c>
+      <c r="E2400" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2400" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2401" s="7">
+        <v>44517.858563877315</v>
+      </c>
+      <c r="B2401" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2401" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D2401" s="2">
+        <v>818110174</v>
+      </c>
+      <c r="E2401" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2401" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2402" s="7">
+        <v>44517.858597777777</v>
+      </c>
+      <c r="B2402" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2402" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D2402" s="2">
+        <v>818142492</v>
+      </c>
+      <c r="E2402" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2402" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2403" s="7">
+        <v>44517.859222488427</v>
+      </c>
+      <c r="B2403" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2403" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2403" s="2">
+        <v>818134194</v>
+      </c>
+      <c r="E2403" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2403" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2404" s="7">
+        <v>44517.85928931713</v>
+      </c>
+      <c r="B2404" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2404" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2404" s="2">
+        <v>818133133</v>
+      </c>
+      <c r="E2404" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2404" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2405" s="7">
+        <v>44517.859412488426</v>
+      </c>
+      <c r="B2405" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C2405" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2405" s="2">
+        <v>821221454</v>
+      </c>
+      <c r="E2405" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2405" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2406" s="7">
+        <v>44517.859517743054</v>
+      </c>
+      <c r="B2406" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2406" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2406" s="2">
+        <v>820143895</v>
+      </c>
+      <c r="E2406" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2406" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2407" s="7">
+        <v>44517.859524386571</v>
+      </c>
+      <c r="B2407" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2407" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2407" s="2">
+        <v>820136449</v>
+      </c>
+      <c r="E2407" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2407" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2408" s="7">
+        <v>44517.85967524306</v>
+      </c>
+      <c r="B2408" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2408" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2408" s="2">
+        <v>818113513</v>
+      </c>
+      <c r="E2408" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2408" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2409" s="7">
+        <v>44517.859689699078</v>
+      </c>
+      <c r="B2409" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2409" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2409" s="2">
+        <v>821237791</v>
+      </c>
+      <c r="E2409" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2409" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2410" s="7">
+        <v>44517.859805706015</v>
+      </c>
+      <c r="B2410" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2410" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2410" s="2">
+        <v>818136244</v>
+      </c>
+      <c r="E2410" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2410" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2411" s="7">
+        <v>44517.860056747682</v>
+      </c>
+      <c r="B2411" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2411" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2411" s="2">
+        <v>819143522</v>
+      </c>
+      <c r="E2411" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2411" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2412" s="7">
+        <v>44517.860206805555</v>
+      </c>
+      <c r="B2412" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2412" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2412" s="2">
+        <v>82027591</v>
+      </c>
+      <c r="E2412" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2412" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2413" s="7">
+        <v>44517.860320729167</v>
+      </c>
+      <c r="B2413" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2413" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2413" s="2">
+        <v>818130950</v>
+      </c>
+      <c r="E2413" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2413" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2414" s="7">
+        <v>44517.860354722223</v>
+      </c>
+      <c r="B2414" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2414" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2414" s="2">
+        <v>81810960</v>
+      </c>
+      <c r="E2414" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2414" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2415" s="7">
+        <v>44517.860910752315</v>
+      </c>
+      <c r="B2415" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2415" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2415" s="2">
+        <v>819227133</v>
+      </c>
+      <c r="E2415" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2415" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2416" s="7">
+        <v>44517.861028275467</v>
+      </c>
+      <c r="B2416" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2416" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2416" s="2">
+        <v>818137249</v>
+      </c>
+      <c r="E2416" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2416" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2417" s="7">
+        <v>44517.861117233799</v>
+      </c>
+      <c r="B2417" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2417" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2417" s="2">
+        <v>81815657</v>
+      </c>
+      <c r="E2417" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2417" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2418" s="7">
+        <v>44517.861336655093</v>
+      </c>
+      <c r="B2418" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2418" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2418" s="2">
+        <v>818126299</v>
+      </c>
+      <c r="E2418" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2418" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2419" s="7">
+        <v>44517.861464675923</v>
+      </c>
+      <c r="B2419" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2419" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D2419" s="2">
+        <v>81810966</v>
+      </c>
+      <c r="E2419" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2419" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2420" s="7">
+        <v>44517.861534467593</v>
+      </c>
+      <c r="B2420" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2420" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2420" s="2">
+        <v>818116264</v>
+      </c>
+      <c r="E2420" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2420" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2421" s="7">
+        <v>44517.861718819448</v>
+      </c>
+      <c r="B2421" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2421" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2421" s="2">
+        <v>820141492</v>
+      </c>
+      <c r="E2421" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2421" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2422" s="7">
+        <v>44517.862151828704</v>
+      </c>
+      <c r="B2422" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2422" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2422" s="2">
+        <v>818236054</v>
+      </c>
+      <c r="E2422" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2422" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2423" s="7">
+        <v>44517.862614386569</v>
+      </c>
+      <c r="B2423" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2423" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2423" s="2">
+        <v>818143920</v>
+      </c>
+      <c r="E2423" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2423" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2424" s="7">
+        <v>44517.862942002314</v>
+      </c>
+      <c r="B2424" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2424" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2424" s="2">
+        <v>818128471</v>
+      </c>
+      <c r="E2424" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2424" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2425" s="7">
+        <v>44517.863622002318</v>
+      </c>
+      <c r="B2425" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2425" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2425" s="2">
+        <v>819149357</v>
+      </c>
+      <c r="E2425" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2425" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2426" s="7">
+        <v>44517.863752881945</v>
+      </c>
+      <c r="B2426" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2426" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D2426" s="2">
+        <v>821237310</v>
+      </c>
+      <c r="E2426" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2426" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2427" s="7">
+        <v>44517.864716493059</v>
+      </c>
+      <c r="B2427" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2427" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2427" s="2">
+        <v>819227746</v>
+      </c>
+      <c r="E2427" s="3">
+        <v>36286</v>
+      </c>
+      <c r="F2427" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2428" s="7">
+        <v>44517.86502002315</v>
+      </c>
+      <c r="B2428" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2428" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D2428" s="2">
+        <v>818125550</v>
+      </c>
+      <c r="E2428" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2428" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2429" s="7">
+        <v>44517.865972349537</v>
+      </c>
+      <c r="B2429" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C2429" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D2429" s="2">
+        <v>81819500</v>
+      </c>
+      <c r="E2429" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2429" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2430" s="7">
+        <v>44517.868780543984</v>
+      </c>
+      <c r="B2430" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2430" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2430" s="2">
+        <v>820148203</v>
+      </c>
+      <c r="E2430" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2430" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2431" s="7">
+        <v>44517.873796712964</v>
+      </c>
+      <c r="B2431" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2431" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2431" s="2">
+        <v>81820173</v>
+      </c>
+      <c r="E2431" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2431" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2432" s="7">
+        <v>44517.881950729163</v>
+      </c>
+      <c r="B2432" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2432" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2432" s="2">
+        <v>818140652</v>
+      </c>
+      <c r="E2432" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2432" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2433" s="7">
+        <v>44517.884429756945</v>
+      </c>
+      <c r="B2433" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2433" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2433" s="2">
+        <v>81814035390831</v>
+      </c>
+      <c r="E2433" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2433" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2434" s="7">
+        <v>44517.884989479164</v>
+      </c>
+      <c r="B2434" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2434" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2434" s="2">
+        <v>818123651</v>
+      </c>
+      <c r="E2434" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2434" s="2" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2435" s="7">
+        <v>44517.886773437502</v>
+      </c>
+      <c r="B2435" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2435" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="D2435" s="2">
+        <v>81823855</v>
+      </c>
+      <c r="E2435" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2435" s="2" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2436" s="7">
+        <v>44517.888546875001</v>
+      </c>
+      <c r="B2436" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2436" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2436" s="2">
+        <v>819145821</v>
+      </c>
+      <c r="E2436" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2436" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2437" s="7">
+        <v>44517.889111296296</v>
+      </c>
+      <c r="B2437" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2437" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2437" s="2">
+        <v>819159962</v>
+      </c>
+      <c r="E2437" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2437" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2438" s="7">
+        <v>44517.889281967597</v>
+      </c>
+      <c r="B2438" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2438" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D2438" s="2">
+        <v>819148633</v>
+      </c>
+      <c r="E2438" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2438" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2439" s="7">
+        <v>44517.897063715282</v>
+      </c>
+      <c r="B2439" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2439" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2439" s="2">
+        <v>818125674</v>
+      </c>
+      <c r="E2439" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2439" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2440" s="7">
+        <v>44517.901535787038</v>
+      </c>
+      <c r="B2440" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2440" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2440" s="2">
+        <v>818133945</v>
+      </c>
+      <c r="E2440" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2440" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2441" s="7">
+        <v>44517.910889918981</v>
+      </c>
+      <c r="B2441" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C2441" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D2441" s="2">
+        <v>818113167</v>
+      </c>
+      <c r="E2441" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2441" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2442" s="7">
+        <v>44517.918363831021</v>
+      </c>
+      <c r="B2442" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2442" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2442" s="2">
+        <v>818117731</v>
+      </c>
+      <c r="E2442" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2442" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2443" s="7">
+        <v>44517.923408356481</v>
+      </c>
+      <c r="B2443" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2443" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2443" s="2">
+        <v>818121060</v>
+      </c>
+      <c r="E2443" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2443" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2444" s="7">
+        <v>44517.951689560185</v>
+      </c>
+      <c r="B2444" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2444" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D2444" s="2">
+        <v>818144624</v>
+      </c>
+      <c r="E2444" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2444" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2445" s="7">
+        <v>44517.965795567128</v>
+      </c>
+      <c r="B2445" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2445" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D2445" s="2">
+        <v>818124382</v>
+      </c>
+      <c r="E2445" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2445" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2446" s="7">
+        <v>44517.979337627316</v>
+      </c>
+      <c r="B2446" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2446" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2446" s="2">
+        <v>818129142</v>
+      </c>
+      <c r="E2446" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2446" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2447" s="7">
+        <v>44518.002509421298</v>
+      </c>
+      <c r="B2447" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2447" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2447" s="2">
+        <v>818135433</v>
+      </c>
+      <c r="E2447" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2447" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2448" s="7">
+        <v>44518.72639434028</v>
+      </c>
+      <c r="B2448" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2448" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2448" s="2">
+        <v>81819599</v>
+      </c>
+      <c r="E2448" s="3">
+        <v>44517</v>
+      </c>
+      <c r="F2448" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2449" s="7">
+        <v>44524.845768043982</v>
+      </c>
+      <c r="B2449" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2449" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D2449" s="2">
+        <v>818136575</v>
+      </c>
+      <c r="E2449" s="3">
+        <v>44524</v>
+      </c>
+      <c r="F2449" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2450" s="7">
+        <v>44524.846364687503</v>
+      </c>
+      <c r="B2450" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2450" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2450" s="2">
+        <v>819142037</v>
+      </c>
+      <c r="E2450" s="3">
+        <v>44524</v>
+      </c>
+      <c r="F2450" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2451" s="7">
+        <v>44524.846732604172</v>
+      </c>
+      <c r="B2451" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2451" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2451" s="2">
+        <v>818231417</v>
+      </c>
+      <c r="E2451" s="3">
+        <v>44524</v>
+      </c>
+      <c r="F2451" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2452" s="7">
+        <v>44524.899765162038</v>
+      </c>
+      <c r="B2452" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2452" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D2452" s="2">
+        <v>818144624</v>
+      </c>
+      <c r="E2452" s="3">
+        <v>44524</v>
+      </c>
+      <c r="F2452" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F2369" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F2452" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{25BF9AEC-6AF4-40B5-9B09-EFFFE67B0424}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{13F12EAD-C763-4533-AABC-1B0310D4A0A2}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="A1:F2469" xr:uid="{5F5CC771-097B-40A8-93C9-60FF357BB416}"/>
+      <autoFilter ref="A1:F2552" xr:uid="{1D1CAD4F-F402-4201-BD04-54E727C54945}"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>

</xml_diff>